<commit_message>
new enhancement in Indoor_Processor.js also Instore_response_builder.py, removed time_delay from request send method
</commit_message>
<xml_diff>
--- a/Transaction_request/XLS/card_data_sanity.xlsx
+++ b/Transaction_request/XLS/card_data_sanity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ganesh\Meijer\Automation_tool\Miejer_Petro\Transaction_request\XLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ganesh\Meijer\Automation_tool\Automation\Transaction_request\XLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="292" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="292" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -5052,8 +5052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O171"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -9337,7 +9337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>